<commit_message>
Now WHERE statements with AND supported, as well as numerical comparisons.
</commit_message>
<xml_diff>
--- a/data/Test.xlsx
+++ b/data/Test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="225" windowWidth="21660" windowHeight="11850" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5380" yWindow="220" windowWidth="21660" windowHeight="11860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>One</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>"MOM"</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -426,9 +429,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -468,12 +471,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -481,7 +487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -492,7 +498,7 @@
         <v>3.141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -503,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -514,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -527,5 +533,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multiple tables using "getJoins()". Still need to do "WHERE xxx.yyy = www.zzz" (not working yet)
</commit_message>
<xml_diff>
--- a/data/Test.xlsx
+++ b/data/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="220" windowWidth="21660" windowHeight="11860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5380" yWindow="220" windowWidth="21660" windowHeight="11860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>One</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>"And Dad"</t>
+  </si>
+  <si>
+    <t>"foobar"</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -454,6 +460,34 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Inner JOIN appears to be working now
</commit_message>
<xml_diff>
--- a/data/Test.xlsx
+++ b/data/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="220" windowWidth="21660" windowHeight="11860" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="800" windowWidth="21660" windowHeight="11860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>One</t>
   </si>
@@ -46,9 +46,6 @@
     <t>"Hi"</t>
   </si>
   <si>
-    <t>"MOM"</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -56,6 +53,15 @@
   </si>
   <si>
     <t>"foobar"</t>
+  </si>
+  <si>
+    <t>"Dad"</t>
+  </si>
+  <si>
+    <t>"Mom"</t>
+  </si>
+  <si>
+    <t>Column_3</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -470,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -484,9 +490,37 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
     </row>
@@ -502,17 +536,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -520,8 +554,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,19 +568,25 @@
       <c r="C2">
         <v>3.141</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -553,8 +596,11 @@
       <c r="C4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -563,6 +609,23 @@
       </c>
       <c r="C5">
         <v>6</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>